<commit_message>
several minor corrections to ids and QA
</commit_message>
<xml_diff>
--- a/ePICreator/Biktarvy.xlsx
+++ b/ePICreator/Biktarvy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/vulcan-eproduct-info/ePICreator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/gravitate-health/ePICreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB53109-EFB4-B24A-877D-D1E0589689F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0179488-6A37-0346-A165-7878241B80DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="19200" windowHeight="21100" firstSheet="6" activeTab="9" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="7" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="152">
   <si>
     <t>id</t>
   </si>
@@ -337,12 +337,6 @@
   </si>
   <si>
     <t>100000072062</t>
-  </si>
-  <si>
-    <t>eu</t>
-  </si>
-  <si>
-    <t>European Union</t>
   </si>
   <si>
     <t>100000072084</t>
@@ -815,6 +809,12 @@
 &lt;p&gt;Biktarvy comes in bottles of 30 tablets and in packs made up of 3 bottles, each containing 30 tablets.
 Each bottle contains a silica gel desiccant that must be kept in the bottle to help protect your tablets.
 The silica gel desiccant is contained in a separate sachet or canister and should not be swallowed.&lt;/p&gt;    </t>
+  </si>
+  <si>
+    <t>GBR</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
   </si>
 </sst>
 </file>
@@ -962,7 +962,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -979,7 +979,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1336,10 +1336,10 @@
     <row r="2" spans="1:13">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>25</v>
@@ -1357,28 +1357,28 @@
         <v>28</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="K2" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>119</v>
       </c>
       <c r="M2" s="10"/>
     </row>
     <row r="3" spans="1:13">
       <c r="B3" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F3" s="8">
         <v>220000000032</v>
@@ -1390,16 +1390,16 @@
         <v>28</v>
       </c>
       <c r="I3" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>108</v>
-      </c>
       <c r="K3" s="10" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -1412,8 +1412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B05DE958-7C5A-B14B-9983-3CEB258B5640}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H3" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1478,11 +1478,9 @@
     <row r="2" spans="1:16" ht="409.6">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>112</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C2" s="8"/>
       <c r="D2" s="3" t="s">
         <v>45</v>
       </c>
@@ -1490,34 +1488,34 @@
         <v>47</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="L2" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="K2" s="6" t="s">
+      <c r="M2" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="N2" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>151</v>
       </c>
       <c r="P2" s="6"/>
     </row>
@@ -1577,10 +1575,10 @@
         <v>40</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1593,8 +1591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C620B326-AC2F-7D41-952C-D15C634902DC}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1644,10 +1642,10 @@
     <row r="2" spans="1:11">
       <c r="A2" s="11"/>
       <c r="B2" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>31</v>
@@ -1656,7 +1654,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>37</v>
@@ -1665,10 +1663,10 @@
         <v>96</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1851,10 +1849,10 @@
     <row r="2" spans="1:13">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -1881,10 +1879,10 @@
     <row r="3" spans="1:13">
       <c r="A3" s="1"/>
       <c r="B3" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1911,10 +1909,10 @@
     <row r="4" spans="1:13">
       <c r="A4" s="1"/>
       <c r="B4" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1941,10 +1939,10 @@
     <row r="5" spans="1:13">
       <c r="A5" s="1"/>
       <c r="B5" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -1959,10 +1957,10 @@
     <row r="6" spans="1:13">
       <c r="A6" s="1"/>
       <c r="B6" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -1977,10 +1975,10 @@
     <row r="7" spans="1:13">
       <c r="A7" s="1"/>
       <c r="B7" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
         <v>17</v>
@@ -2024,7 +2022,7 @@
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2107,34 +2105,34 @@
     <row r="2" spans="1:19" ht="19">
       <c r="A2" s="11"/>
       <c r="B2" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="E2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>129</v>
-      </c>
       <c r="I2" s="10" t="s">
-        <v>97</v>
+        <v>150</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>98</v>
+        <v>151</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>83</v>
@@ -2146,7 +2144,7 @@
         <v>55</v>
       </c>
       <c r="O2" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:19">
@@ -2274,22 +2272,22 @@
     <row r="2" spans="1:9">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F2" s="8">
         <v>100000073665</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H2" s="13">
         <v>200000002152</v>
@@ -2361,16 +2359,16 @@
     <row r="2" spans="1:11" ht="18">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F2" s="8">
         <v>10219000</v>
@@ -2378,7 +2376,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="18"/>
       <c r="I2" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J2" s="8">
         <v>20053000</v>
@@ -2491,16 +2489,16 @@
     <row r="2" spans="1:23">
       <c r="A2" s="1"/>
       <c r="B2" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
         <v>32</v>
@@ -2509,13 +2507,13 @@
         <v>100000155527</v>
       </c>
       <c r="H2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I2" s="8">
         <v>654321</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K2" s="13">
         <v>100000073504</v>
@@ -2524,7 +2522,7 @@
         <v>1</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="N2" s="13">
         <v>200000003529</v>

</xml_diff>

<commit_message>
composition category and packaging
</commit_message>
<xml_diff>
--- a/ePICreator/Biktarvy.xlsx
+++ b/ePICreator/Biktarvy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/gravitate-health/ePICreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0179488-6A37-0346-A165-7878241B80DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7929F7CD-2B9E-A648-9379-91E44DACBAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="4" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="7" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="153">
   <si>
     <t>id</t>
   </si>
@@ -815,6 +815,9 @@
   </si>
   <si>
     <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>country</t>
   </si>
 </sst>
 </file>
@@ -1591,7 +1594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C620B326-AC2F-7D41-952C-D15C634902DC}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -2021,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5EB2795-F6E7-D149-BA96-099EC7B435E4}">
   <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2072,7 +2075,7 @@
         <v>23</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
+        <v>152</v>
       </c>
       <c r="K1" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
create new packaging method
</commit_message>
<xml_diff>
--- a/ePICreator/Biktarvy.xlsx
+++ b/ePICreator/Biktarvy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaoalmeida/Desktop/hl7Europe/gravitate/gravitate-health/ePICreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FAF3BF-8BC5-9642-B367-73B4378E372F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F8CE8A-A58B-F74D-8B50-97CD3952696D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="10" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="7" xr2:uid="{0EBB815D-796F-C248-AC7C-E52173F2F74B}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="7" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="166">
   <si>
     <t>id</t>
   </si>
@@ -1179,6 +1179,12 @@
 Carrigtohill
 County Cork
 Irlanda&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>30 tablets</t>
+  </si>
+  <si>
+    <t>Biktarvy 50 mg/200 mg/25 mg film-coated tablets 30 (1 bottle of 30) film-coated tablets</t>
   </si>
 </sst>
 </file>
@@ -1933,7 +1939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB4B3880-CBCE-B242-93DB-BF401DA7FB8A}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -2800,10 +2806,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{185E689D-306D-3A44-A772-E9755EF7D37C}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2938,6 +2944,47 @@
         <v>200000003529</v>
       </c>
     </row>
+    <row r="3" spans="1:23">
+      <c r="B3" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="2">
+        <v>100000155527</v>
+      </c>
+      <c r="H3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I3" s="8">
+        <v>654321</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="K3" s="13">
+        <v>100000073504</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="N3" s="13">
+        <v>200000003529</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>